<commit_message>
fixed locations + added locatorpage
</commit_message>
<xml_diff>
--- a/_site/sections/apps/Speurtocht/locations.xlsx
+++ b/_site/sections/apps/Speurtocht/locations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahirmas\Git Projects\janohirmas.github.io\sections\apps\Speurtocht\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E6A1AE7-1ECC-49B8-A7AD-5E00EFE35229}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C1DA4A-F944-4F85-AD27-F0A862971180}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2263" yWindow="2263" windowWidth="16457" windowHeight="8966" xr2:uid="{0F739182-30D5-4CBF-BBD9-9195ADBA7024}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="12549" xr2:uid="{0F739182-30D5-4CBF-BBD9-9195ADBA7024}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>Home</t>
   </si>
@@ -60,21 +60,9 @@
     <t>Alfajores</t>
   </si>
   <si>
-    <t>Fit4Free</t>
-  </si>
-  <si>
-    <t>Clandestine Dancing</t>
-  </si>
-  <si>
     <t>Westerpark</t>
   </si>
   <si>
-    <t>Schinkelhaven</t>
-  </si>
-  <si>
-    <t> 4.9342416</t>
-  </si>
-  <si>
     <t>Yoga</t>
   </si>
   <si>
@@ -90,9 +78,6 @@
     <t>Next Clue</t>
   </si>
   <si>
-    <t>Answer</t>
-  </si>
-  <si>
     <t>Waar blijft je jong en je kan je stretchen tot in de breedste zin van het woord?</t>
   </si>
   <si>
@@ -103,6 +88,27 @@
   </si>
   <si>
     <t>Bart Smit</t>
+  </si>
+  <si>
+    <t>Golf</t>
+  </si>
+  <si>
+    <t>Daar waar de stenen rollen, En we draaien tot we tollen, Wanneer de klok zijn uren slaat, maar pas op wel in de maat</t>
+  </si>
+  <si>
+    <t>Het is tijd nu voor iets zoet. Iets zo goed, dat de konigin hebben moet</t>
+  </si>
+  <si>
+    <t>en laten we voor het laatst gaan waar het allemaal begon. Let op: Die die teruggaat, die die een fout maakt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">De kippen gaan op stok. Ik snap er geen bal van. Maar we zitten op dezelfde golflengte. Jij hebt een lekkere glow. Het wordt nu black in het light. </t>
+  </si>
+  <si>
+    <t>dancing</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/dir/52.4007811,4.934678/'52.397076,4.931854'/'52.391499,4.934217'/'52.384724,4.93048'/'52.385614,4.914406'/'52.383925,4.901745'/'52.3755256,4.8949212'/'52.373983,4.891038'/'52.384574,4.886282'/'52.386214,4.872481'/@52.3866547,4.8860201,14z/data=!3m1!4b1!4m41!4m40!1m0!1m5!1m1!1s0x0:0xd12f3756d87c2a7f!2m2!1d4.9317984!2d52.3969183!1m3!2m2!1d4.934217!2d52.391499!1m3!2m2!1d4.93048!2d52.384724!1m3!2m2!1d4.914406!2d52.385614!1m3!2m2!1d4.901745!2d52.383925!1m3!2m2!1d4.8949212!2d52.3755256!1m3!2m2!1d4.891038!2d52.373983!1m3!2m2!1d4.886282!2d52.384574!1m3!2m2!1d4.872481!2d52.386214!3e1</t>
   </si>
 </sst>
 </file>
@@ -110,8 +116,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="0.000000"/>
-    <numFmt numFmtId="170" formatCode="0.0000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -159,13 +165,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -482,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{352834DD-120F-44F4-9BDD-4C14260529BD}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -493,9 +499,8 @@
     <col min="1" max="2" width="17.61328125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.61328125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.84375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.84375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.23046875" style="2"/>
-    <col min="7" max="7" width="50.3046875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="38.765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="50.3046875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -506,212 +511,242 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E1" s="4"/>
-      <c r="F1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="F1" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="6">
-        <v>52.397075999999998</v>
-      </c>
-      <c r="D2" s="6">
-        <v>4.9318540000000004</v>
+        <v>18</v>
+      </c>
+      <c r="C2" s="7">
+        <v>52.400781100000003</v>
+      </c>
+      <c r="D2" s="1">
+        <v>4.9346779999999999</v>
       </c>
       <c r="E2" s="6" t="str">
         <f>+"{latitude: "&amp;C2&amp;", longitude: "&amp;D2&amp;"},"</f>
+        <v>{latitude: 52.4007811, longitude: 4.934678},</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="1" t="str">
+        <f>+C2&amp;","&amp;D2</f>
+        <v>52.4007811,4.934678</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="6">
+        <v>52.397075999999998</v>
+      </c>
+      <c r="D3" s="6">
+        <v>4.9318540000000004</v>
+      </c>
+      <c r="E3" s="6" t="str">
+        <f>+"{latitude: "&amp;C3&amp;", longitude: "&amp;D3&amp;"},"</f>
         <v>{latitude: 52.397076, longitude: 4.931854},</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="F3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="1" t="str">
+        <f t="shared" ref="G3:G11" si="0">+C3&amp;","&amp;D3</f>
+        <v>52.397076,4.931854</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="6">
-        <v>52.3915747</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="6" t="str">
-        <f t="shared" ref="E3:E12" si="0">+"{latitude: "&amp;C3&amp;", longitude: "&amp;D3&amp;"},"</f>
-        <v>{latitude: 52.3915747, longitude:  4.9342416},</v>
-      </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="C4" s="6">
-        <v>52.384723999999999</v>
-      </c>
-      <c r="D4" s="6">
-        <v>4.9304800000000002</v>
+        <v>52.391499000000003</v>
+      </c>
+      <c r="D4" s="4">
+        <v>4.9342170000000003</v>
       </c>
       <c r="E4" s="6" t="str">
+        <f t="shared" ref="E4:E10" si="1">+"{latitude: "&amp;C4&amp;", longitude: "&amp;D4&amp;"},"</f>
+        <v>{latitude: 52.391499, longitude: 4.934217},</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>{latitude: 52.384724, longitude: 4.93048},</v>
-      </c>
-      <c r="F4" s="4"/>
+        <v>52.391499,4.934217</v>
+      </c>
     </row>
     <row r="5" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="C5" s="6">
-        <v>52.385613999999997</v>
+        <v>52.384723999999999</v>
       </c>
       <c r="D5" s="6">
-        <v>4.9144059999999996</v>
+        <v>4.9304800000000002</v>
       </c>
       <c r="E5" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>{latitude: 52.384724, longitude: 4.93048},</v>
+      </c>
+      <c r="G5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>{latitude: 52.385614, longitude: 4.914406},</v>
-      </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="7" t="s">
-        <v>16</v>
+        <v>52.384724,4.93048</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="6">
+        <v>52.385613999999997</v>
+      </c>
+      <c r="D6" s="6">
+        <v>4.9144059999999996</v>
+      </c>
+      <c r="E6" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>{latitude: 52.385614, longitude: 4.914406},</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>52.385614,4.914406</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C7" s="4">
         <v>52.383924999999998</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D7" s="4">
         <v>4.901745</v>
       </c>
-      <c r="E6" s="6" t="str">
+      <c r="E7" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>{latitude: 52.383925, longitude: 4.901745},</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>{latitude: 52.383925, longitude: 4.901745},</v>
-      </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="7"/>
-    </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A7" s="4" t="s">
+        <v>52.383925,4.901745</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="1">
+      <c r="B8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1">
         <v>52.375525600000003</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D8" s="1">
         <v>4.8949211999999998</v>
       </c>
-      <c r="E7" s="6" t="str">
+      <c r="E8" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>{latitude: 52.3755256, longitude: 4.8949212},</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>{latitude: 52.3755256, longitude: 4.8949212},</v>
-      </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="4" t="s">
+        <v>52.3755256,4.8949212</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C9" s="4">
         <v>52.373983000000003</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D9" s="4">
         <v>4.891038</v>
       </c>
-      <c r="E8" s="6" t="str">
+      <c r="E9" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>{latitude: 52.373983, longitude: 4.891038},</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>{latitude: 52.373983, longitude: 4.891038},</v>
-      </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="7"/>
-    </row>
-    <row r="9" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="4" t="s">
+        <v>52.373983,4.891038</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="8">
+        <v>52.384574000000001</v>
+      </c>
+      <c r="D10" s="6">
+        <v>4.8862819999999996</v>
+      </c>
+      <c r="E10" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>{latitude: 52.384574, longitude: 4.886282},</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>52.384574,4.886282</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="C9" s="4">
-        <v>52.381337000000002</v>
-      </c>
-      <c r="D9" s="4">
-        <v>4.8912789999999999</v>
-      </c>
-      <c r="E9" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>{latitude: 52.381337, longitude: 4.891279},</v>
-      </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="7"/>
-    </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="8">
-        <v>52.384407000000003</v>
-      </c>
-      <c r="D10" s="6">
-        <v>4.8860720000000004</v>
-      </c>
-      <c r="E10" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>{latitude: 52.384407, longitude: 4.886072},</v>
-      </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="7"/>
-    </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="C11" s="4">
         <v>52.386214000000002</v>
@@ -723,28 +758,26 @@
         <f>+"{latitude: "&amp;C11&amp;", longitude: "&amp;D11&amp;"},"</f>
         <v>{latitude: 52.386214, longitude: 4.872481},</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="7"/>
+      <c r="F11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>52.386214,4.872481</v>
+      </c>
     </row>
     <row r="12" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="4">
-        <v>52.354655000000001</v>
-      </c>
-      <c r="D12" s="4">
-        <v>4.8552309999999999</v>
-      </c>
-      <c r="E12" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>{latitude: 52.354655, longitude: 4.855231},</v>
-      </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="7"/>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A14" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>